<commit_message>
improvde docstrings & comments, esp. for dfba_bound_scale_factor
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/dfba_test_model.xlsx
+++ b/tests/submodels/fixtures/dfba_test_model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/submodels/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20380" yWindow="1660" windowWidth="20000" windowHeight="13840" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="-17340" yWindow="460" windowWidth="17200" windowHeight="13940" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -2020,7 +2020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
@@ -2281,14 +2281,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
ensure that exchange reactions satisfy the “s ->” form; make dfba_test_model.xlsx do this; fix the hand solutions accordingly
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/dfba_test_model.xlsx
+++ b/tests/submodels/fixtures/dfba_test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-17340" yWindow="460" windowWidth="17200" windowHeight="13940" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="-20360" yWindow="920" windowWidth="19840" windowHeight="13980" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -483,24 +483,15 @@
     <t>ex_m1</t>
   </si>
   <si>
-    <t>[c]:  ==&gt; m1</t>
-  </si>
-  <si>
     <t>1 / second</t>
   </si>
   <si>
     <t>ex_m2</t>
   </si>
   <si>
-    <t>[c]:  ==&gt; m2</t>
-  </si>
-  <si>
     <t>ex_m3</t>
   </si>
   <si>
-    <t>[c]:  ==&gt; m3</t>
-  </si>
-  <si>
     <t>r1</t>
   </si>
   <si>
@@ -796,6 +787,15 @@
   </si>
   <si>
     <t>molar / second</t>
+  </si>
+  <si>
+    <t>[c]: m1 ==&gt;</t>
+  </si>
+  <si>
+    <t>[c]: m2 ==&gt;</t>
+  </si>
+  <si>
+    <t>[c]: m3 ==&gt;</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -887,6 +887,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1667,14 +1671,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="14" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="14" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1771,22 +1779,22 @@
         <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>136</v>
+        <v>238</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1.6605390671738471E-22</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1.9926468806086161E-22</v>
+        <v>136</v>
+      </c>
+      <c r="G4">
+        <v>-1.9926468806086161E-22</v>
+      </c>
+      <c r="H4">
+        <v>-1.6605390671738471E-22</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1796,29 +1804,29 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>139</v>
+        <v>239</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1.6605390671738471E-22</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1.9926468806086161E-22</v>
+        <v>136</v>
+      </c>
+      <c r="G5">
+        <v>-1.9926468806086161E-22</v>
+      </c>
+      <c r="H5">
+        <v>-1.6605390671738471E-22</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1828,29 +1836,29 @@
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>141</v>
+        <v>240</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="3">
+        <v>136</v>
+      </c>
+      <c r="G6" s="7">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="7">
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1860,20 +1868,20 @@
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1886,20 +1894,20 @@
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1912,20 +1920,20 @@
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1938,20 +1946,20 @@
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1982,11 +1990,11 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="F4:F10 I4:I6">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G4:G10">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G6:G10">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="H4:H10">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="H6:H10">
       <formula1>-1E-100</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molar / second&quot; or blank." sqref="I7:I10">
@@ -2038,7 +2046,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2060,10 +2068,10 @@
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>87</v>
@@ -2092,21 +2100,21 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -2116,21 +2124,21 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -2140,21 +2148,21 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -2164,21 +2172,21 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -2188,21 +2196,21 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -2212,21 +2220,21 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -2281,9 +2289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2296,7 +2304,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2327,10 +2335,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>39</v>
@@ -2350,20 +2358,20 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>38</v>
@@ -2434,7 +2442,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2460,7 +2468,7 @@
         <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>39</v>
@@ -2480,14 +2488,14 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>75</v>
@@ -2544,7 +2552,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2555,7 +2563,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2576,7 +2584,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>110</v>
@@ -2605,11 +2613,11 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>107</v>
@@ -2618,7 +2626,7 @@
         <v>-1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -2689,7 +2697,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2716,7 +2724,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>67</v>
@@ -2748,7 +2756,7 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -2767,7 +2775,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2777,7 +2785,7 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2794,7 +2802,7 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2811,7 +2819,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2828,7 +2836,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2845,7 +2853,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2862,7 +2870,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2879,7 +2887,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2896,7 +2904,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2961,7 +2969,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3044,7 +3052,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3077,42 +3085,42 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
@@ -3129,7 +3137,7 @@
         <v>81</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>67</v>
@@ -3138,10 +3146,10 @@
         <v>87</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>48</v>
@@ -3153,19 +3161,19 @@
         <v>58</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>30</v>
@@ -3297,7 +3305,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3433,7 +3441,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3449,7 +3457,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>39</v>
@@ -3499,7 +3507,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3523,10 +3531,10 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -3546,7 +3554,7 @@
         <v>81</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>67</v>
@@ -3573,10 +3581,10 @@
         <v>46</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3641,7 +3649,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3669,46 +3677,46 @@
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>39</v>
@@ -3795,7 +3803,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3817,28 +3825,28 @@
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>39</v>
@@ -3910,7 +3918,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3940,25 +3948,25 @@
         <v>87</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>39</v>
@@ -3976,10 +3984,10 @@
         <v>46</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test expected species adjustments, fix hand solutions and expected adjustments through test IV; catch and workaround strange problem in unit tests, presumably caused by obj_table's shared related attributes
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/dfba_test_model.xlsx
+++ b/tests/submodels/fixtures/dfba_test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20360" yWindow="920" windowWidth="19840" windowHeight="13980" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="-31560" yWindow="460" windowWidth="31540" windowHeight="12620" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="242">
   <si>
     <t>!!!ObjTables schema='wc_lang' objTablesVersion='1.0.14' date='2020-11-19 16:20:20'</t>
   </si>
@@ -796,6 +796,9 @@
   </si>
   <si>
     <t>[c]: m3 ==&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  </t>
   </si>
 </sst>
 </file>
@@ -1671,18 +1674,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6:H6"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="14" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="14" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1693,7 +1698,9 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>241</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -2030,7 +2037,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2429,9 +2436,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2552,12 +2559,14 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="11" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4206,7 +4215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>

<commit_message>
in preparation for using WC Lang code that splits reversible reactions in dFBA submodels, mark these reactions as reversible:, ex_m1, ex_m2, r1, and r2. they all have bounds or rate laws for both directions
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/dfba_test_model.xlsx
+++ b/tests/submodels/fixtures/dfba_test_model.xlsx
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31560" yWindow="460" windowWidth="31540" windowHeight="12620" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="-16520" yWindow="460" windowWidth="16500" windowHeight="8080" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="760" yWindow="5100" windowWidth="28160" windowHeight="9480" tabRatio="500" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -885,15 +886,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,6 +1203,7 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1480,6 +1482,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1563,6 +1566,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1676,8 +1680,9 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4:G5"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1718,13 +1723,13 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>128</v>
       </c>
       <c r="J2" s="4"/>
@@ -1789,7 +1794,7 @@
         <v>238</v>
       </c>
       <c r="E4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>136</v>
@@ -1821,7 +1826,7 @@
         <v>239</v>
       </c>
       <c r="E5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>136</v>
@@ -1858,10 +1863,10 @@
       <c r="F6" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>0</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -2039,6 +2044,9 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2277,6 +2285,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2300,6 +2309,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2438,8 +2448,9 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2561,6 +2572,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2697,6 +2709,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2969,6 +2982,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3052,6 +3066,7 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3093,42 +3108,42 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>189</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="7" t="s">
         <v>191</v>
       </c>
       <c r="U2" s="4"/>
@@ -3296,6 +3311,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3441,6 +3457,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3507,6 +3524,7 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3539,10 +3557,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>202</v>
       </c>
       <c r="I2" s="4"/>
@@ -3649,6 +3667,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3803,6 +3822,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3918,6 +3938,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4070,6 +4091,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4141,6 +4163,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4219,6 +4242,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4311,6 +4335,7 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4351,29 +4376,29 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>57</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="Q2" s="4"/>
@@ -4615,6 +4640,7 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4643,22 +4669,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>80</v>
       </c>
       <c r="I2" s="4"/>
@@ -4895,6 +4921,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5178,6 +5205,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
more of in preparation for using WC Lang code that splits reversible reactions in dFBA submodels, mark these reactions as reversible:, ex_m1, ex_m2, r1, and r2. they all have bounds or rate laws for both directions
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/dfba_test_model.xlsx
+++ b/tests/submodels/fixtures/dfba_test_model.xlsx
@@ -10,7 +10,6 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-16520" yWindow="460" windowWidth="16500" windowHeight="8080" firstSheet="10" activeTab="11"/>
-    <workbookView xWindow="760" yWindow="5100" windowWidth="28160" windowHeight="9480" tabRatio="500" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1203,7 +1202,6 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1482,7 +1480,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1566,7 +1563,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1680,9 +1676,8 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A10"/>
     </sheetView>
-    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2044,9 +2039,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2309,7 +2301,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2450,7 +2441,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2572,7 +2562,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2709,7 +2698,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2982,7 +2970,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3066,7 +3053,6 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3311,7 +3297,6 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3457,7 +3442,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3524,7 +3508,6 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3667,7 +3650,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3822,7 +3804,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3938,7 +3919,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4091,7 +4071,6 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4163,7 +4142,6 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4242,7 +4220,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4335,7 +4312,6 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4640,7 +4616,6 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4921,7 +4896,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5205,7 +5179,6 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
revise for models with only irreversible reactions, as made when reactions were split by SplitReversibleReactionsTransform in PrepForWcSimTransform; enables great simplification of determine_bounds(); simplify by not bounding individual reactions to stop species populations from going negative in the next time step -- just use separate constraints that prevent this; ensure that all reactions are irreversible; unify treatment of pseudo-reactions; set correct reversible attributes for rxns in dfba_test_model.xlsx; skip exception from Validator errors until https://github.com/KarrLab/wc_lang/issues/142 is resolved for fixtures/dfba_test_model.xlsx; simplify by making/using dict. of all wc_lang.DfbaObjReactions; stop warning when exchange reactions don't have the form 's ->'
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/dfba_test_model.xlsx
+++ b/tests/submodels/fixtures/dfba_test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-16520" yWindow="460" windowWidth="16500" windowHeight="8080" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="-17420" yWindow="460" windowWidth="17400" windowHeight="7580" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="243">
   <si>
     <t>!!!ObjTables schema='wc_lang' objTablesVersion='1.0.14' date='2020-11-19 16:20:20'</t>
   </si>
@@ -799,13 +799,16 @@
   </si>
   <si>
     <t xml:space="preserve">                  </t>
+  </si>
+  <si>
+    <t>s^-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -825,6 +828,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -858,10 +866,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -870,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -893,6 +910,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1674,9 +1697,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A10"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1716,7 +1739,7 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="4"/>
       <c r="G2" s="6" t="s">
         <v>128</v>
@@ -2037,7 +2060,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2120,8 +2143,8 @@
       <c r="F3" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>136</v>
+      <c r="G3" s="8" t="s">
+        <v>242</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -4308,9 +4331,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
no changes to model
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/dfba_test_model.xlsx
+++ b/tests/submodels/fixtures/dfba_test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-17420" yWindow="460" windowWidth="17400" windowHeight="7580" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="-17600" yWindow="460" windowWidth="17400" windowHeight="7160" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -866,19 +866,10 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -887,7 +878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -913,9 +904,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1697,9 +1685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1727,7 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="9"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="6" t="s">
         <v>128</v>
@@ -3318,7 +3306,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4241,7 +4229,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4331,9 +4319,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>